<commit_message>
update prototype_4a,this closes #3
</commit_message>
<xml_diff>
--- a/planning/prototype_4a.xlsx
+++ b/planning/prototype_4a.xlsx
@@ -1,17 +1,31 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="20225"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10810"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/EduardoFrancisco/Desktop/4a/planning/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3060DB6-79CE-4945-87B4-ADBACB3E7644}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22360" windowHeight="14240" tabRatio="990" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="22360" windowHeight="14240" tabRatio="990" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loc_Methods" sheetId="1" r:id="rId1"/>
     <sheet name="Chapter_Pages" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -187,11 +201,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -233,13 +247,19 @@
     <font>
       <b/>
       <sz val="10"/>
-      <color rgb="FF000000"/>
+      <color theme="0"/>
       <name val="Times New Roman"/>
       <family val="1"/>
-      <charset val="161"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -256,6 +276,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF70AD47"/>
         <bgColor rgb="FF339966"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0070C0"/>
+        <bgColor rgb="FFFFFF00"/>
       </patternFill>
     </fill>
   </fills>
@@ -344,7 +370,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -415,8 +441,11 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -492,6 +521,14 @@
       <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -816,14 +853,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AMK25"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="8.83203125" style="1"/>
     <col min="2" max="2" width="15.1640625" style="1" customWidth="1"/>
@@ -835,7 +872,7 @@
     <col min="8" max="1025" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="18" customHeight="1">
+    <row r="1" spans="1:7" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -858,7 +895,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -884,7 +921,7 @@
         <v>1.0196113404699423</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -910,7 +947,7 @@
         <v>1.0196113404699423</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -936,7 +973,7 @@
         <v>0.46410700351241357</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -962,7 +999,7 @@
         <v>0.21728893637694804</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -988,7 +1025,7 @@
         <v>8.364352634996762E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -1014,7 +1051,7 @@
         <v>1.7945346060241649E-5</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -1040,7 +1077,7 @@
         <v>4.7920430752746268E-2</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -1066,7 +1103,7 @@
         <v>7.7337511995958133E-2</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -1092,7 +1129,7 @@
         <v>9.0495367177808636E-2</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30">
+    <row r="11" spans="1:7" ht="34" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -1118,7 +1155,7 @@
         <v>0.11154042701674756</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -1144,7 +1181,7 @@
         <v>0.29432951093937959</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -1170,7 +1207,7 @@
         <v>0.32010508519726777</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -1196,7 +1233,7 @@
         <v>1.4890255348105541</v>
       </c>
     </row>
-    <row r="15" spans="1:7">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" s="15"/>
       <c r="B15" s="16" t="s">
         <v>20</v>
@@ -1216,7 +1253,7 @@
         <v>5.2350339604157359</v>
       </c>
     </row>
-    <row r="16" spans="1:7">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="20"/>
       <c r="B16" s="21" t="s">
         <v>21</v>
@@ -1236,7 +1273,7 @@
         <v>0.40269492003197971</v>
       </c>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B17" s="23"/>
       <c r="C17" s="24"/>
       <c r="D17" s="24"/>
@@ -1244,7 +1281,7 @@
       <c r="F17" s="24"/>
       <c r="G17" s="24"/>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B18" s="19" t="s">
         <v>22</v>
       </c>
@@ -1257,7 +1294,7 @@
       <c r="F18" s="23"/>
       <c r="G18" s="24"/>
     </row>
-    <row r="19" spans="2:7">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B19" s="19" t="s">
         <v>23</v>
       </c>
@@ -1270,13 +1307,13 @@
       <c r="F19" s="23"/>
       <c r="G19" s="24"/>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B20"/>
       <c r="C20"/>
       <c r="E20" s="23"/>
       <c r="F20" s="23"/>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B21" s="19" t="s">
         <v>24</v>
       </c>
@@ -1292,7 +1329,7 @@
         <v>4.395269124478685</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B22" s="19" t="s">
         <v>26</v>
       </c>
@@ -1308,7 +1345,7 @@
         <v>8.5081382493892264</v>
       </c>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B23" s="19" t="s">
         <v>28</v>
       </c>
@@ -1324,7 +1361,7 @@
         <v>16.469620953940066</v>
       </c>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B24" s="19" t="s">
         <v>30</v>
       </c>
@@ -1340,7 +1377,7 @@
         <v>31.881053929269871</v>
       </c>
     </row>
-    <row r="25" spans="2:7">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
       <c r="B25" s="19" t="s">
         <v>32</v>
       </c>
@@ -1367,16 +1404,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I15" sqref="I15"/>
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:6" ht="30">
+    <row r="1" spans="1:6" ht="34" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1396,7 +1433,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="6">
         <v>1</v>
       </c>
@@ -1419,7 +1456,7 @@
         <v>0.22410462994639299</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="11">
         <v>2</v>
       </c>
@@ -1442,7 +1479,7 @@
         <v>4.3033069211018604E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="11">
         <v>3</v>
       </c>
@@ -1465,7 +1502,7 @@
         <v>1.3624016263719349E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="11">
         <v>4</v>
       </c>
@@ -1488,7 +1525,7 @@
         <v>4.3033069211018604E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="11">
         <v>5</v>
       </c>
@@ -1511,7 +1548,7 @@
         <v>1.3624016263719349E-2</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="11">
         <v>6</v>
       </c>
@@ -1534,7 +1571,7 @@
         <v>4.3033069211018604E-3</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="11">
         <v>7</v>
       </c>
@@ -1557,7 +1594,7 @@
         <v>4.3033069211018604E-3</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="11">
         <v>8</v>
       </c>
@@ -1580,7 +1617,7 @@
         <v>4.3033069211018604E-3</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="11">
         <v>9</v>
       </c>
@@ -1603,7 +1640,7 @@
         <v>4.3033069211018604E-3</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="11">
         <v>10</v>
       </c>
@@ -1626,7 +1663,7 @@
         <v>0.11550856670528628</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="24">
+    <row r="12" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A12" s="11">
         <v>11</v>
       </c>
@@ -1649,7 +1686,7 @@
         <v>0.11550856670528628</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="24">
+    <row r="13" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A13" s="11">
         <v>12</v>
       </c>
@@ -1672,7 +1709,7 @@
         <v>0.11550856670528628</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="24">
+    <row r="14" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A14" s="11">
         <v>13</v>
       </c>
@@ -1695,7 +1732,7 @@
         <v>0.33226603332973415</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="24">
+    <row r="15" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A15" s="11">
         <v>14</v>
       </c>
@@ -1718,7 +1755,7 @@
         <v>4.8290183477389927E-2</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="24">
+    <row r="16" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A16" s="11">
         <v>15</v>
       </c>
@@ -1741,7 +1778,7 @@
         <v>0.22190195492324824</v>
       </c>
     </row>
-    <row r="17" spans="1:6" ht="24">
+    <row r="17" spans="1:6" ht="28" x14ac:dyDescent="0.2">
       <c r="A17" s="11">
         <v>16</v>
       </c>
@@ -1764,45 +1801,45 @@
         <v>4.3033069211018604E-3</v>
       </c>
     </row>
-    <row r="18" spans="1:6">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="20"/>
       <c r="B18" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21">
+      <c r="C18" s="29"/>
+      <c r="D18" s="29">
         <f>SUM(D2:D17)</f>
         <v>187</v>
       </c>
-      <c r="E18" s="21">
+      <c r="E18" s="29">
         <f>SUM(E2:E17)</f>
         <v>38.708912869664324</v>
       </c>
-      <c r="F18" s="21">
+      <c r="F18" s="29">
         <f>SUM(F2:F17)</f>
         <v>1.2304596827677758</v>
       </c>
     </row>
-    <row r="19" spans="1:6">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="20"/>
       <c r="B19" s="28" t="s">
         <v>21</v>
       </c>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21">
+      <c r="C19" s="29"/>
+      <c r="D19" s="29">
         <f>D18/$A$17</f>
         <v>11.6875</v>
       </c>
-      <c r="E19" s="21">
+      <c r="E19" s="29">
         <f>E18/A17</f>
         <v>2.4193070543540203</v>
       </c>
-      <c r="F19" s="21">
+      <c r="F19" s="29">
         <f>F18/A17</f>
         <v>7.690373017298599E-2</v>
       </c>
     </row>
-    <row r="21" spans="1:6">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B21" s="19" t="s">
         <v>22</v>
       </c>
@@ -1814,7 +1851,7 @@
       <c r="E21" s="23"/>
       <c r="F21" s="23"/>
     </row>
-    <row r="22" spans="1:6">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B22" s="19" t="s">
         <v>23</v>
       </c>
@@ -1826,14 +1863,14 @@
       <c r="E22" s="23"/>
       <c r="F22" s="23"/>
     </row>
-    <row r="23" spans="1:6">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="23"/>
       <c r="F23" s="23"/>
     </row>
-    <row r="24" spans="1:6">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B24" s="19" t="s">
         <v>24</v>
       </c>
@@ -1850,7 +1887,7 @@
         <v>6.3375179612117245</v>
       </c>
     </row>
-    <row r="25" spans="1:6">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B25" s="19" t="s">
         <v>26</v>
       </c>
@@ -1867,7 +1904,7 @@
         <v>8.43928111212605</v>
       </c>
     </row>
-    <row r="26" spans="1:6">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B26" s="19" t="s">
         <v>28</v>
       </c>
@@ -1884,7 +1921,7 @@
         <v>11.23806924499352</v>
       </c>
     </row>
-    <row r="27" spans="1:6">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B27" s="19" t="s">
         <v>30</v>
       </c>
@@ -1901,7 +1938,7 @@
         <v>14.965042481379408</v>
       </c>
     </row>
-    <row r="28" spans="1:6">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B28" s="19" t="s">
         <v>32</v>
       </c>

</xml_diff>